<commit_message>
Avancement visiuel tableau matriuce compétence.
</commit_message>
<xml_diff>
--- a/Symfony/web/uploads/FichierHierarchieRH/HierarchieRH.xlsx
+++ b/Symfony/web/uploads/FichierHierarchieRH/HierarchieRH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noxingenierie-my.sharepoint.com/personal/l_morisseau_groupe-nox_com/Documents/Partagé avec tout le monde/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="34BA23330D5BADDCE0731695EA14A39035646E17" xr6:coauthVersionLast="17" xr6:coauthVersionMax="17" xr10:uidLastSave="{B54EB9D4-951C-430A-9EC2-28B1010E584D}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="34BA23330D5BADDCE0731695EA14A39035646E17" xr6:coauthVersionLast="17" xr6:coauthVersionMax="17" xr10:uidLastSave="{9217C8A0-2415-4AB7-A39D-AFBD914C7466}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5157" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5158" uniqueCount="1086">
   <si>
     <t>Matricule</t>
   </si>
@@ -2891,6 +2891,9 @@
   </si>
   <si>
     <t>FIZES</t>
+  </si>
+  <si>
+    <t>SORTIE LE</t>
   </si>
   <si>
     <t>FONTAINE</t>
@@ -3754,8 +3757,8 @@
   <dimension ref="A1:L798"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="C473" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F486" sqref="F486"/>
+      <pane ySplit="1" topLeftCell="C646" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -20520,7 +20523,7 @@
       <c r="G538" s="12" t="s">
         <v>878</v>
       </c>
-      <c r="H538" s="13" t="s">
+      <c r="H538" s="8" t="s">
         <v>842</v>
       </c>
       <c r="I538" s="13" t="s">
@@ -20871,7 +20874,9 @@
         <v>234</v>
       </c>
       <c r="J549" s="8"/>
-      <c r="K549" s="8"/>
+      <c r="K549" s="8" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="550" spans="1:12">
       <c r="A550" s="12">
@@ -20884,7 +20889,7 @@
         <v>868</v>
       </c>
       <c r="D550" s="12" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="E550" s="12" t="s">
         <v>73</v>
@@ -20915,10 +20920,10 @@
         <v>868</v>
       </c>
       <c r="D551" s="12" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E551" s="12" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="F551" s="12" t="s">
         <v>881</v>
@@ -20946,7 +20951,7 @@
         <v>868</v>
       </c>
       <c r="D552" s="12" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E552" s="12" t="s">
         <v>44</v>
@@ -20978,10 +20983,10 @@
         <v>868</v>
       </c>
       <c r="D553" s="12" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="E553" s="12" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="F553" s="12" t="s">
         <v>840</v>
@@ -21012,7 +21017,7 @@
         <v>383</v>
       </c>
       <c r="E554" s="12" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="F554" s="12" t="s">
         <v>881</v>
@@ -21040,7 +21045,7 @@
         <v>868</v>
       </c>
       <c r="D555" s="12" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E555" s="12" t="s">
         <v>758</v>
@@ -21071,7 +21076,7 @@
         <v>868</v>
       </c>
       <c r="D556" s="11" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="E556" s="11" t="s">
         <v>800</v>
@@ -21102,10 +21107,10 @@
         <v>868</v>
       </c>
       <c r="D557" s="12" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="E557" s="12" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="F557" s="12" t="s">
         <v>874</v>
@@ -21133,10 +21138,10 @@
         <v>868</v>
       </c>
       <c r="D558" s="12" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E558" s="12" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="F558" s="12" t="s">
         <v>874</v>
@@ -21164,7 +21169,7 @@
         <v>868</v>
       </c>
       <c r="D559" s="12" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="E559" s="12" t="s">
         <v>47</v>
@@ -21196,13 +21201,13 @@
         <v>868</v>
       </c>
       <c r="D560" s="11" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="E560" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F560" s="11" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="G560" s="11" t="s">
         <v>233</v>
@@ -21227,7 +21232,7 @@
         <v>868</v>
       </c>
       <c r="D561" s="12" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E561" s="12" t="s">
         <v>65</v>
@@ -21258,10 +21263,10 @@
         <v>868</v>
       </c>
       <c r="D562" s="12" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="E562" s="12" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="F562" s="12" t="s">
         <v>855</v>
@@ -21290,7 +21295,7 @@
         <v>868</v>
       </c>
       <c r="D563" s="12" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="E563" s="12" t="s">
         <v>143</v>
@@ -21322,10 +21327,10 @@
         <v>868</v>
       </c>
       <c r="D564" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E564" s="11" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F564" s="11" t="s">
         <v>842</v>
@@ -21354,10 +21359,10 @@
         <v>868</v>
       </c>
       <c r="D565" s="12" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E565" s="12" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F565" s="12" t="s">
         <v>842</v>
@@ -21369,7 +21374,7 @@
         <v>842</v>
       </c>
       <c r="I565" s="13" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="J565" s="13"/>
       <c r="K565" s="13"/>
@@ -21386,10 +21391,10 @@
         <v>868</v>
       </c>
       <c r="D566" s="11" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="E566" s="11" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F566" s="11" t="s">
         <v>842</v>
@@ -21417,7 +21422,7 @@
         <v>868</v>
       </c>
       <c r="D567" s="12" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="E567" s="12" t="s">
         <v>101</v>
@@ -21449,10 +21454,10 @@
         <v>868</v>
       </c>
       <c r="D568" s="12" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="E568" s="12" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F568" s="12" t="s">
         <v>881</v>
@@ -21480,7 +21485,7 @@
         <v>868</v>
       </c>
       <c r="D569" s="12" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="E569" s="12" t="s">
         <v>429</v>
@@ -21512,10 +21517,10 @@
         <v>868</v>
       </c>
       <c r="D570" s="11" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="E570" s="11" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F570" s="11" t="s">
         <v>842</v>
@@ -21544,7 +21549,7 @@
         <v>868</v>
       </c>
       <c r="D571" s="12" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="E571" s="12" t="s">
         <v>101</v>
@@ -21553,7 +21558,7 @@
         <v>855</v>
       </c>
       <c r="G571" s="12" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="H571" s="13" t="s">
         <v>842</v>
@@ -21576,7 +21581,7 @@
         <v>868</v>
       </c>
       <c r="D572" s="12" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="E572" s="12" t="s">
         <v>623</v>
@@ -21608,10 +21613,10 @@
         <v>868</v>
       </c>
       <c r="D573" s="12" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E573" s="12" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="F573" s="12" t="s">
         <v>874</v>
@@ -21639,7 +21644,7 @@
         <v>868</v>
       </c>
       <c r="D574" s="12" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E574" s="12" t="s">
         <v>612</v>
@@ -21671,10 +21676,10 @@
         <v>868</v>
       </c>
       <c r="D575" s="12" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E575" s="12" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="F575" s="12" t="s">
         <v>874</v>
@@ -21702,10 +21707,10 @@
         <v>868</v>
       </c>
       <c r="D576" s="12" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E576" s="12" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="F576" s="12" t="s">
         <v>881</v>
@@ -21733,10 +21738,10 @@
         <v>868</v>
       </c>
       <c r="D577" s="12" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E577" s="12" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="F577" s="12" t="s">
         <v>840</v>
@@ -21764,7 +21769,7 @@
         <v>868</v>
       </c>
       <c r="D578" s="12" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E578" s="12" t="s">
         <v>101</v>
@@ -21796,10 +21801,10 @@
         <v>868</v>
       </c>
       <c r="D579" s="12" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="E579" s="12" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="F579" s="12" t="s">
         <v>874</v>
@@ -21827,10 +21832,10 @@
         <v>868</v>
       </c>
       <c r="D580" s="12" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E580" s="12" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F580" s="12" t="s">
         <v>874</v>
@@ -21858,7 +21863,7 @@
         <v>868</v>
       </c>
       <c r="D581" s="12" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E581" s="12" t="s">
         <v>473</v>
@@ -21889,10 +21894,10 @@
         <v>868</v>
       </c>
       <c r="D582" s="12" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="E582" s="12" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F582" s="12" t="s">
         <v>855</v>
@@ -21921,7 +21926,7 @@
         <v>868</v>
       </c>
       <c r="D583" s="12" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E583" s="12" t="s">
         <v>105</v>
@@ -21953,10 +21958,10 @@
         <v>868</v>
       </c>
       <c r="D584" s="12" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E584" s="12" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F584" s="12" t="s">
         <v>874</v>
@@ -21984,7 +21989,7 @@
         <v>868</v>
       </c>
       <c r="D585" s="12" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E585" s="12" t="s">
         <v>323</v>
@@ -22015,10 +22020,10 @@
         <v>868</v>
       </c>
       <c r="D586" s="12" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E586" s="12" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="F586" s="12" t="s">
         <v>874</v>
@@ -22046,7 +22051,7 @@
         <v>868</v>
       </c>
       <c r="D587" s="12" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="E587" s="12" t="s">
         <v>47</v>
@@ -22078,7 +22083,7 @@
         <v>868</v>
       </c>
       <c r="D588" s="12" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E588" s="12" t="s">
         <v>572</v>
@@ -22110,7 +22115,7 @@
         <v>868</v>
       </c>
       <c r="D589" s="12" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E589" s="12" t="s">
         <v>165</v>
@@ -22141,7 +22146,7 @@
         <v>868</v>
       </c>
       <c r="D590" s="12" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="E590" s="12" t="s">
         <v>47</v>
@@ -22172,10 +22177,10 @@
         <v>868</v>
       </c>
       <c r="D591" s="12" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E591" s="12" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="F591" s="12" t="s">
         <v>874</v>
@@ -22203,10 +22208,10 @@
         <v>868</v>
       </c>
       <c r="D592" s="12" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E592" s="12" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="F592" s="12" t="s">
         <v>842</v>
@@ -22235,7 +22240,7 @@
         <v>868</v>
       </c>
       <c r="D593" s="12" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E593" s="12" t="s">
         <v>861</v>
@@ -22299,10 +22304,10 @@
         <v>868</v>
       </c>
       <c r="D595" s="12" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="E595" s="12" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="F595" s="12" t="s">
         <v>874</v>
@@ -22393,10 +22398,10 @@
         <v>868</v>
       </c>
       <c r="D598" s="12" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="E598" s="12" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="F598" s="12" t="s">
         <v>855</v>
@@ -22425,10 +22430,10 @@
         <v>868</v>
       </c>
       <c r="D599" s="12" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="E599" s="12" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="F599" s="12" t="s">
         <v>881</v>
@@ -22456,7 +22461,7 @@
         <v>868</v>
       </c>
       <c r="D600" s="12" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="E600" s="12" t="s">
         <v>52</v>
@@ -22488,10 +22493,10 @@
         <v>868</v>
       </c>
       <c r="D601" s="12" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="E601" s="12" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="F601" s="12" t="s">
         <v>881</v>
@@ -22519,10 +22524,10 @@
         <v>868</v>
       </c>
       <c r="D602" s="12" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="E602" s="12" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="F602" s="12" t="s">
         <v>881</v>
@@ -22559,7 +22564,7 @@
         <v>874</v>
       </c>
       <c r="G603" s="12" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="H603" s="8" t="s">
         <v>842</v>
@@ -22581,10 +22586,10 @@
         <v>868</v>
       </c>
       <c r="D604" s="12" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E604" s="12" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F604" s="12" t="s">
         <v>855</v>
@@ -22613,10 +22618,10 @@
         <v>868</v>
       </c>
       <c r="D605" s="12" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E605" s="12" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="F605" s="12" t="s">
         <v>855</v>
@@ -22645,7 +22650,7 @@
         <v>868</v>
       </c>
       <c r="D606" s="12" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="E606" s="12" t="s">
         <v>856</v>
@@ -22709,7 +22714,7 @@
         <v>868</v>
       </c>
       <c r="D608" s="12" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E608" s="12" t="s">
         <v>19</v>
@@ -22740,7 +22745,7 @@
         <v>868</v>
       </c>
       <c r="D609" s="12" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="E609" s="12" t="s">
         <v>570</v>
@@ -22771,10 +22776,10 @@
         <v>868</v>
       </c>
       <c r="D610" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="E610" s="11" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="F610" s="11" t="s">
         <v>842</v>
@@ -22803,7 +22808,7 @@
         <v>868</v>
       </c>
       <c r="D611" s="12" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="E611" s="12" t="s">
         <v>429</v>
@@ -22834,7 +22839,7 @@
         <v>868</v>
       </c>
       <c r="D612" s="12" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="E612" s="12" t="s">
         <v>73</v>
@@ -22865,10 +22870,10 @@
         <v>868</v>
       </c>
       <c r="D613" s="12" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="E613" s="12" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="F613" s="12" t="s">
         <v>874</v>
@@ -22896,7 +22901,7 @@
         <v>868</v>
       </c>
       <c r="D614" s="12" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="E614" s="12" t="s">
         <v>212</v>
@@ -22927,7 +22932,7 @@
         <v>868</v>
       </c>
       <c r="D615" s="12" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="E615" s="12" t="s">
         <v>76</v>
@@ -22958,7 +22963,7 @@
         <v>868</v>
       </c>
       <c r="D616" s="12" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="E616" s="12" t="s">
         <v>257</v>
@@ -22989,7 +22994,7 @@
         <v>868</v>
       </c>
       <c r="D617" s="12" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="E617" s="12" t="s">
         <v>355</v>
@@ -23020,10 +23025,10 @@
         <v>868</v>
       </c>
       <c r="D618" s="12" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="E618" s="12" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="F618" s="12" t="s">
         <v>881</v>
@@ -23051,10 +23056,10 @@
         <v>868</v>
       </c>
       <c r="D619" s="12" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="E619" s="12" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="F619" s="12" t="s">
         <v>881</v>
@@ -23082,16 +23087,16 @@
         <v>868</v>
       </c>
       <c r="D620" s="12" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="E620" s="12" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="F620" s="12" t="s">
         <v>865</v>
       </c>
       <c r="G620" s="12" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="H620" s="13" t="s">
         <v>842</v>
@@ -23114,10 +23119,10 @@
         <v>868</v>
       </c>
       <c r="D621" s="11" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="E621" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="F621" s="11" t="s">
         <v>842</v>
@@ -23146,7 +23151,7 @@
         <v>868</v>
       </c>
       <c r="D622" s="12" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="E622" s="12" t="s">
         <v>530</v>
@@ -23177,7 +23182,7 @@
         <v>868</v>
       </c>
       <c r="D623" s="12" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="E623" s="12" t="s">
         <v>446</v>
@@ -23209,7 +23214,7 @@
         <v>868</v>
       </c>
       <c r="D624" s="12" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E624" s="12" t="s">
         <v>508</v>
@@ -23240,10 +23245,10 @@
         <v>868</v>
       </c>
       <c r="D625" s="12" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="E625" s="12" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="F625" s="12" t="s">
         <v>855</v>
@@ -23272,10 +23277,10 @@
         <v>868</v>
       </c>
       <c r="D626" s="11" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="E626" s="11" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="F626" s="11" t="s">
         <v>842</v>
@@ -23303,7 +23308,7 @@
         <v>868</v>
       </c>
       <c r="D627" s="12" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="E627" s="12" t="s">
         <v>429</v>
@@ -23334,7 +23339,7 @@
         <v>868</v>
       </c>
       <c r="D628" s="12" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="E628" s="12" t="s">
         <v>85</v>
@@ -23365,7 +23370,7 @@
         <v>868</v>
       </c>
       <c r="D629" s="12" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="E629" s="12" t="s">
         <v>508</v>
@@ -23397,10 +23402,10 @@
         <v>868</v>
       </c>
       <c r="D630" s="12" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="E630" s="12" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="F630" s="12" t="s">
         <v>874</v>
@@ -23429,10 +23434,10 @@
         <v>868</v>
       </c>
       <c r="D631" s="12" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="E631" s="12" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="F631" s="12" t="s">
         <v>855</v>
@@ -23461,10 +23466,10 @@
         <v>868</v>
       </c>
       <c r="D632" s="12" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="E632" s="12" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="F632" s="12" t="s">
         <v>865</v>
@@ -23493,7 +23498,7 @@
         <v>868</v>
       </c>
       <c r="D633" s="12" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="E633" s="12" t="s">
         <v>429</v>
@@ -23522,10 +23527,10 @@
         <v>838</v>
       </c>
       <c r="C634" s="26" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="D634" s="26" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="E634" s="26" t="s">
         <v>131</v>
@@ -23554,13 +23559,13 @@
         <v>838</v>
       </c>
       <c r="C635" s="26" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="D635" s="26" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="E635" s="26" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="F635" s="26" t="s">
         <v>874</v>
@@ -23585,10 +23590,10 @@
         <v>838</v>
       </c>
       <c r="C636" s="12" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="D636" s="12" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E636" s="12" t="s">
         <v>406</v>
@@ -23617,7 +23622,7 @@
         <v>745</v>
       </c>
       <c r="D637" s="12" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="E637" s="12" t="s">
         <v>719</v>
@@ -23648,7 +23653,7 @@
         <v>87</v>
       </c>
       <c r="D638" s="12" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="E638" s="12" t="s">
         <v>71</v>
@@ -23679,7 +23684,7 @@
         <v>745</v>
       </c>
       <c r="D639" s="12" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="E639" s="12" t="s">
         <v>572</v>
@@ -23710,7 +23715,7 @@
         <v>658</v>
       </c>
       <c r="D640" s="12" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E640" s="12" t="s">
         <v>124</v>
@@ -23739,10 +23744,10 @@
         <v>617</v>
       </c>
       <c r="D641" s="7" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="E641" s="7" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="F641" s="7" t="s">
         <v>620</v>
@@ -23768,7 +23773,7 @@
         <v>745</v>
       </c>
       <c r="D642" s="12" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="E642" s="12" t="s">
         <v>191</v>
@@ -23797,10 +23802,10 @@
         <v>557</v>
       </c>
       <c r="D643" s="12" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="E643" s="12" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="F643" s="12" t="s">
         <v>560</v>
@@ -23826,7 +23831,7 @@
         <v>810</v>
       </c>
       <c r="D644" s="11" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="E644" s="11" t="s">
         <v>131</v>
@@ -23855,7 +23860,7 @@
         <v>658</v>
       </c>
       <c r="D645" s="16" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="E645" s="16" t="s">
         <v>623</v>

</xml_diff>